<commit_message>
level 1 script complete
</commit_message>
<xml_diff>
--- a/6res.xlsx
+++ b/6res.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="38">
   <si>
     <t>UID</t>
   </si>
@@ -62,6 +62,72 @@
   </si>
   <si>
     <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>A21</t>
+  </si>
+  <si>
+    <t>A22</t>
+  </si>
+  <si>
+    <t>A23</t>
+  </si>
+  <si>
+    <t>A24</t>
   </si>
 </sst>
 </file>
@@ -393,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,6 +552,644 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>1875</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5">
+        <v>1875</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>1875</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <v>1875</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>1875</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9">
+        <v>1875</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10">
+        <v>1875</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11">
+        <v>1875</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12">
+        <v>1875</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13">
+        <v>1875</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14">
+        <v>1875</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15">
+        <v>1875</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16">
+        <v>1875</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17">
+        <v>1875</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18">
+        <v>1875</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19">
+        <v>1875</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20">
+        <v>1875</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21">
+        <v>1875</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22">
+        <v>1875</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23">
+        <v>1875</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24">
+        <v>1875</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25">
+        <v>1875</v>
+      </c>
+      <c r="I25" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Backup before adding volumetric ratio variation reactions
</commit_message>
<xml_diff>
--- a/6res.xlsx
+++ b/6res.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
   <si>
     <t>UID</t>
   </si>
@@ -62,6 +62,24 @@
   </si>
   <si>
     <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
   </si>
 </sst>
 </file>
@@ -393,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,6 +504,180 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>1875</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5">
+        <v>1875</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>1875</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <v>1875</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>1875</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9">
+        <v>1875</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Backup before MoClo code restructure
</commit_message>
<xml_diff>
--- a/6res.xlsx
+++ b/6res.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="20">
   <si>
     <t>UID</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
   </si>
 </sst>
 </file>
@@ -399,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -515,7 +521,7 @@
         <v>16</v>
       </c>
       <c r="H4">
-        <v>2875</v>
+        <v>1875</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
@@ -544,9 +550,67 @@
         <v>17</v>
       </c>
       <c r="H5">
+        <v>2875</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6">
         <v>2625</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <v>1875</v>
+      </c>
+      <c r="I7" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added backbones to document
</commit_message>
<xml_diff>
--- a/6res.xlsx
+++ b/6res.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>UID</t>
   </si>
@@ -62,18 +62,6 @@
   </si>
   <si>
     <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A6</t>
   </si>
 </sst>
 </file>
@@ -405,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -492,125 +480,9 @@
         <v>15</v>
       </c>
       <c r="H3">
-        <v>2625</v>
+        <v>2875</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4">
-        <v>1875</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5">
-        <v>2875</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6">
-        <v>2625</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7">
-        <v>1875</v>
-      </c>
-      <c r="I7" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Backup before import design and part overhaul
</commit_message>
<xml_diff>
--- a/6res.xlsx
+++ b/6res.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>UID</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
   </si>
 </sst>
 </file>
@@ -393,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -480,9 +486,67 @@
         <v>15</v>
       </c>
       <c r="H3">
+        <v>2625</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
         <v>2875</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5">
+        <v>2625</v>
+      </c>
+      <c r="I5" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>